<commit_message>
Alterar iloc por loc
</commit_message>
<xml_diff>
--- a/Saldo_guide.xlsx
+++ b/Saldo_guide.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lauro.telles\Desktop\Mesa_app_3\app_mesa_de_opera-es_corrigido\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{831EA9ED-B920-4507-B07C-28557D44BE76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A0F30A2-6DCC-44C8-9339-72CE1A1400F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{6D531EE6-2FB1-45E6-B6C9-5F5D184A839C}"/>
+    <workbookView xWindow="21480" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{6D531EE6-2FB1-45E6-B6C9-5F5D184A839C}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -3265,10 +3265,13 @@
   <dimension ref="A1:CJ310"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="20.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:88" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>